<commit_message>
Complete hotel booking system with Telr payment integration
Features:
- Custom city search API integration
- Hotel search and details with availability editor
- Guest details modification with room-by-room configuration
- Telr payment gateway integration (AED currency)
- Backend API for bookings and wishlist
- Responsive mobile-first design
- Complete payment flow with success/failure/cancel pages
</commit_message>
<xml_diff>
--- a/backend/wishlist.xlsx
+++ b/backend/wishlist.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,69 +488,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>WL00001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>fd1ec1e0-9efb-4f05-b34d-54ad48753537</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>60954</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Al Maha Arjaan By Rotana</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Fatima bint Mubarak Street, Abu Dhabi, AE</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Abu Dhabi</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://i.travelapi.com/lodging/1000000/920000/910800/910720/dead5c34_z.jpg</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>{"checkIn": "2025-11-04", "checkOut": "2025-11-07", "guests": "2", "adults": "2", "children": "0", "rooms": "1", "childrenAges": "", "roomGuests": ""}</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2025-10-24 12:34:25</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>